<commit_message>
new rules for May
</commit_message>
<xml_diff>
--- a/db-processing-rules/src/main/resources/SOLOR LOINC Rules.xlsx
+++ b/db-processing-rules/src/main/resources/SOLOR LOINC Rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="765" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="638" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="362">
   <si>
     <t>ID</t>
   </si>
@@ -757,15 +757,361 @@
   </si>
   <si>
     <t>urea nitrogen measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Measles virus Ag</t>
+  </si>
+  <si>
+    <t>measles antigen assay (procedure)</t>
+  </si>
+  <si>
+    <t>Chlamydia trachomatis rRNA</t>
+  </si>
+  <si>
+    <t>Chlamydia trachomatis ribosomal ribonucleic acid assay (procedure)</t>
+  </si>
+  <si>
+    <t>Cytomegalovirus DNA</t>
+  </si>
+  <si>
+    <t>cytomegalovirus deoxyribonucleic acid assay (procedure)</t>
+  </si>
+  <si>
+    <t>Temazepam</t>
+  </si>
+  <si>
+    <t>temazepam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Mumps virus Ag</t>
+  </si>
+  <si>
+    <t>mumps virus antigen assay (procedure)</t>
+  </si>
+  <si>
+    <t>Chromium</t>
+  </si>
+  <si>
+    <t>chromium measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>iron measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Methamphetamine</t>
+  </si>
+  <si>
+    <t>methamphetamine measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Borrelia burgdorferi Ab</t>
+  </si>
+  <si>
+    <t>measurement of Borrelia burgdorferi antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
+    <t>copper measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Cryptococcus sp Ag</t>
+  </si>
+  <si>
+    <t>Cryptococcus species antigen assay (procedure)</t>
+  </si>
+  <si>
+    <t>N-desalkylflurazepam</t>
+  </si>
+  <si>
+    <t>N-Desalkylflurazepam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Phenobarbital</t>
+  </si>
+  <si>
+    <t>phenobarbital measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Cadmium</t>
+  </si>
+  <si>
+    <t>cadmium measurement (procedure)</t>
+  </si>
+  <si>
+    <t>HIV 1 Ab</t>
+  </si>
+  <si>
+    <t>measurement of Human immunodeficiency virus 1 antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Influenza virus A Ab</t>
+  </si>
+  <si>
+    <t>influenza A antibody level (procedure)</t>
+  </si>
+  <si>
+    <t>Adenovirus Ag</t>
+  </si>
+  <si>
+    <t>Adenovirus antigen assay (procedure)</t>
+  </si>
+  <si>
+    <t>Flurazepam</t>
+  </si>
+  <si>
+    <t>flurazepam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Rubella virus Ag</t>
+  </si>
+  <si>
+    <t>rubella virus antigen assay (procedure)</t>
+  </si>
+  <si>
+    <t>Morphine</t>
+  </si>
+  <si>
+    <t>measurement of morphine (procedure)</t>
+  </si>
+  <si>
+    <t>Triglyceride</t>
+  </si>
+  <si>
+    <t>triglycerides measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Reagin Ab</t>
+  </si>
+  <si>
+    <t>Treponema pallidum reagin antibody level (procedure)</t>
+  </si>
+  <si>
+    <t>Pneumocystis jiroveci Ag</t>
+  </si>
+  <si>
+    <t>Pneumocystis jirovecii antigen assay (procedure)</t>
+  </si>
+  <si>
+    <t>Coccidioides immitis Ab</t>
+  </si>
+  <si>
+    <t>measurement of Coccidioides immitis antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Bicarbonate</t>
+  </si>
+  <si>
+    <t>bicarbonate measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>selenium measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Triazolam</t>
+  </si>
+  <si>
+    <t>triazolam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Nickel</t>
+  </si>
+  <si>
+    <t>nickel measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Clonazepam</t>
+  </si>
+  <si>
+    <t>clonazepam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>DNA double strand Ab</t>
+  </si>
+  <si>
+    <t>antibody to double stranded deoxyribonucleic acid measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Histoplasma capsulatum Ag</t>
+  </si>
+  <si>
+    <t>Histoplasma capsulatum antigen assay (procedure)</t>
+  </si>
+  <si>
+    <t>Borrelia burgdorferi Ab.IgG</t>
+  </si>
+  <si>
+    <t>Borrelia burgdorferi immunoglobulin G level (procedure)</t>
+  </si>
+  <si>
+    <t>Methaqualone</t>
+  </si>
+  <si>
+    <t>methaqualone measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Amobarbital</t>
+  </si>
+  <si>
+    <t>amobarbital measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Carboxy tetrahydrocannabinol</t>
+  </si>
+  <si>
+    <t>carboxy tetrahydrocannabinol measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Secobarbital</t>
+  </si>
+  <si>
+    <t>secobarbital measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Urobilinogen</t>
+  </si>
+  <si>
+    <t>urobilin measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Pentobarbital</t>
+  </si>
+  <si>
+    <t>pentobarbital measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Testosterone</t>
+  </si>
+  <si>
+    <t>testosterone measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Oxycodone</t>
+  </si>
+  <si>
+    <t>oxycodone measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Cobalt</t>
+  </si>
+  <si>
+    <t>cobalt measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Alpha hydroxyalprazolam</t>
+  </si>
+  <si>
+    <t>alpha-Hydroxyalprazolam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Butalbital</t>
+  </si>
+  <si>
+    <t>butalbital measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Acetaminophen</t>
+  </si>
+  <si>
+    <t>acetaminophen measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Herpes simplex virus Ag</t>
+  </si>
+  <si>
+    <t>Herpes simplex virus antigen assay (procedure)</t>
+  </si>
+  <si>
+    <t>Codeine</t>
+  </si>
+  <si>
+    <t>codeine measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Parvovirus B19 DNA</t>
+  </si>
+  <si>
+    <t>parvovirus B19 deoxyribonucleic acid assay (procedure)</t>
+  </si>
+  <si>
+    <t>Meperidine</t>
+  </si>
+  <si>
+    <t>meperidine measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Cortisol.free</t>
+  </si>
+  <si>
+    <t>cortisol, free measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>aluminum measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Blastomyces dermatitidis Ab</t>
+  </si>
+  <si>
+    <t>measurement of Blastomyces dermatitidis antibody (procedure)</t>
+  </si>
+  <si>
+    <t>6-Monoacetylmorphine</t>
+  </si>
+  <si>
+    <t>6-Monoacetylmorphine measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Cotinine</t>
+  </si>
+  <si>
+    <t>cotinine measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Saint Louis encephalitis virus Ab</t>
+  </si>
+  <si>
+    <t>measurement of Saint Louis encephalitis virus antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Methylenedioxyamphetamine</t>
+  </si>
+  <si>
+    <t>methylenedioxyamphetamine measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Midazolam</t>
+  </si>
+  <si>
+    <t>midazolam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Western equine encephalitis virus Ab</t>
+  </si>
+  <si>
+    <t>measurement of Western equine encephalitis virus antibody (procedure)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="D\-MMM\-YY;@"/>
+    <numFmt numFmtId="166" formatCode="D\-MMM\-YY;@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -791,17 +1137,17 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -938,7 +1284,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -962,17 +1308,25 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -980,7 +1334,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -996,19 +1350,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1184,7 +1538,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1192,15 +1546,41 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Normal_LOINC Rules" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Normal_LOINC Rules" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_LOINC Rules" xfId="22" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1387,16 +1767,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BB101"/>
+  <dimension ref="A1:BB166"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A167" activeCellId="0" sqref="A167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.53441295546559"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.53441295546559"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="4" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.8542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.4251012145749"/>
@@ -6869,6 +7250,1946 @@
       </c>
       <c r="L101" s="50"/>
     </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="56"/>
+      <c r="B102" s="57"/>
+      <c r="C102" s="57"/>
+      <c r="D102" s="58"/>
+      <c r="E102" s="56"/>
+      <c r="F102" s="56"/>
+      <c r="G102" s="56"/>
+      <c r="H102" s="56"/>
+      <c r="I102" s="56"/>
+      <c r="J102" s="56"/>
+      <c r="K102" s="59"/>
+    </row>
+    <row r="103" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="50" t="n">
+        <v>2051</v>
+      </c>
+      <c r="B103" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C103" s="60"/>
+      <c r="D103" s="52"/>
+      <c r="E103" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F103" s="61" t="s">
+        <v>247</v>
+      </c>
+      <c r="G103" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H103" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I103" s="50" t="n">
+        <v>398518009</v>
+      </c>
+      <c r="J103" s="50" t="s">
+        <v>248</v>
+      </c>
+      <c r="K103" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="50" t="n">
+        <v>2052</v>
+      </c>
+      <c r="B104" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C104" s="60"/>
+      <c r="D104" s="52"/>
+      <c r="E104" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F104" s="61" t="s">
+        <v>249</v>
+      </c>
+      <c r="G104" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H104" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I104" s="50" t="n">
+        <v>122322003</v>
+      </c>
+      <c r="J104" s="50" t="s">
+        <v>250</v>
+      </c>
+      <c r="K104" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="50" t="n">
+        <v>2053</v>
+      </c>
+      <c r="B105" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C105" s="60"/>
+      <c r="D105" s="52"/>
+      <c r="E105" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F105" s="61" t="s">
+        <v>251</v>
+      </c>
+      <c r="G105" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H105" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I105" s="50" t="n">
+        <v>122325001</v>
+      </c>
+      <c r="J105" s="50" t="s">
+        <v>252</v>
+      </c>
+      <c r="K105" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="50" t="n">
+        <v>2054</v>
+      </c>
+      <c r="B106" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C106" s="60"/>
+      <c r="D106" s="52"/>
+      <c r="E106" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F106" s="61" t="s">
+        <v>253</v>
+      </c>
+      <c r="G106" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H106" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I106" s="50" t="n">
+        <v>121691007</v>
+      </c>
+      <c r="J106" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="K106" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="50" t="n">
+        <v>2055</v>
+      </c>
+      <c r="B107" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C107" s="60"/>
+      <c r="D107" s="52"/>
+      <c r="E107" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F107" s="61" t="s">
+        <v>255</v>
+      </c>
+      <c r="G107" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H107" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I107" s="50" t="n">
+        <v>74040009</v>
+      </c>
+      <c r="J107" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="K107" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="50" t="n">
+        <v>2056</v>
+      </c>
+      <c r="B108" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C108" s="60"/>
+      <c r="D108" s="52"/>
+      <c r="E108" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F108" s="61" t="s">
+        <v>256</v>
+      </c>
+      <c r="G108" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H108" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I108" s="50" t="n">
+        <v>122355008</v>
+      </c>
+      <c r="J108" s="50" t="s">
+        <v>257</v>
+      </c>
+      <c r="K108" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="50" t="n">
+        <v>2057</v>
+      </c>
+      <c r="B109" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C109" s="60"/>
+      <c r="D109" s="52"/>
+      <c r="E109" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F109" s="61" t="s">
+        <v>258</v>
+      </c>
+      <c r="G109" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H109" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I109" s="50" t="n">
+        <v>72244009</v>
+      </c>
+      <c r="J109" s="50" t="s">
+        <v>259</v>
+      </c>
+      <c r="K109" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="50" t="n">
+        <v>2058</v>
+      </c>
+      <c r="B110" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C110" s="60"/>
+      <c r="D110" s="52"/>
+      <c r="E110" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F110" s="61" t="s">
+        <v>260</v>
+      </c>
+      <c r="G110" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H110" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I110" s="50" t="n">
+        <v>42950004</v>
+      </c>
+      <c r="J110" s="50" t="s">
+        <v>261</v>
+      </c>
+      <c r="K110" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="50" t="n">
+        <v>2059</v>
+      </c>
+      <c r="B111" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C111" s="60"/>
+      <c r="D111" s="52"/>
+      <c r="E111" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F111" s="61" t="s">
+        <v>262</v>
+      </c>
+      <c r="G111" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H111" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I111" s="50" t="n">
+        <v>27965000</v>
+      </c>
+      <c r="J111" s="50" t="s">
+        <v>263</v>
+      </c>
+      <c r="K111" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="50" t="n">
+        <v>2060</v>
+      </c>
+      <c r="B112" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C112" s="60"/>
+      <c r="D112" s="52"/>
+      <c r="E112" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F112" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="G112" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H112" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I112" s="50" t="n">
+        <v>104277002</v>
+      </c>
+      <c r="J112" s="50" t="s">
+        <v>265</v>
+      </c>
+      <c r="K112" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="50" t="n">
+        <v>2061</v>
+      </c>
+      <c r="B113" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C113" s="60"/>
+      <c r="D113" s="52"/>
+      <c r="E113" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F113" s="61" t="s">
+        <v>266</v>
+      </c>
+      <c r="G113" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H113" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I113" s="50" t="n">
+        <v>39847004</v>
+      </c>
+      <c r="J113" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="K113" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="50" t="n">
+        <v>2062</v>
+      </c>
+      <c r="B114" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C114" s="60"/>
+      <c r="D114" s="52"/>
+      <c r="E114" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F114" s="61" t="s">
+        <v>268</v>
+      </c>
+      <c r="G114" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H114" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I114" s="50" t="n">
+        <v>121980003</v>
+      </c>
+      <c r="J114" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="K114" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="50" t="n">
+        <v>2063</v>
+      </c>
+      <c r="B115" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C115" s="60"/>
+      <c r="D115" s="52"/>
+      <c r="E115" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F115" s="61" t="s">
+        <v>270</v>
+      </c>
+      <c r="G115" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H115" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I115" s="50" t="n">
+        <v>121389007</v>
+      </c>
+      <c r="J115" s="50" t="s">
+        <v>271</v>
+      </c>
+      <c r="K115" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="50" t="n">
+        <v>2064</v>
+      </c>
+      <c r="B116" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C116" s="60"/>
+      <c r="D116" s="52"/>
+      <c r="E116" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F116" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="G116" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H116" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I116" s="50" t="n">
+        <v>105294009</v>
+      </c>
+      <c r="J116" s="50" t="s">
+        <v>273</v>
+      </c>
+      <c r="K116" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="50" t="n">
+        <v>2065</v>
+      </c>
+      <c r="B117" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C117" s="60"/>
+      <c r="D117" s="52"/>
+      <c r="E117" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F117" s="61" t="s">
+        <v>274</v>
+      </c>
+      <c r="G117" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H117" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I117" s="50" t="n">
+        <v>84266007</v>
+      </c>
+      <c r="J117" s="50" t="s">
+        <v>275</v>
+      </c>
+      <c r="K117" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="50" t="n">
+        <v>2066</v>
+      </c>
+      <c r="B118" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C118" s="60"/>
+      <c r="D118" s="52"/>
+      <c r="E118" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F118" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="G118" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H118" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I118" s="50" t="n">
+        <v>28804003</v>
+      </c>
+      <c r="J118" s="50" t="s">
+        <v>277</v>
+      </c>
+      <c r="K118" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="50" t="n">
+        <v>2067</v>
+      </c>
+      <c r="B119" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C119" s="60"/>
+      <c r="D119" s="52"/>
+      <c r="E119" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F119" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="G119" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H119" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I119" s="50" t="n">
+        <v>28317006</v>
+      </c>
+      <c r="J119" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="K119" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="50" t="n">
+        <v>2068</v>
+      </c>
+      <c r="B120" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C120" s="60"/>
+      <c r="D120" s="52"/>
+      <c r="E120" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F120" s="61" t="s">
+        <v>278</v>
+      </c>
+      <c r="G120" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H120" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I120" s="50" t="n">
+        <v>315142009</v>
+      </c>
+      <c r="J120" s="50" t="s">
+        <v>279</v>
+      </c>
+      <c r="K120" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="50" t="n">
+        <v>2069</v>
+      </c>
+      <c r="B121" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C121" s="60"/>
+      <c r="D121" s="52"/>
+      <c r="E121" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F121" s="61" t="s">
+        <v>280</v>
+      </c>
+      <c r="G121" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H121" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I121" s="50" t="n">
+        <v>121960004</v>
+      </c>
+      <c r="J121" s="50" t="s">
+        <v>281</v>
+      </c>
+      <c r="K121" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="50" t="n">
+        <v>2070</v>
+      </c>
+      <c r="B122" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C122" s="60"/>
+      <c r="D122" s="52"/>
+      <c r="E122" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F122" s="61" t="s">
+        <v>282</v>
+      </c>
+      <c r="G122" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H122" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I122" s="50" t="n">
+        <v>46057001</v>
+      </c>
+      <c r="J122" s="50" t="s">
+        <v>283</v>
+      </c>
+      <c r="K122" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="50" t="n">
+        <v>2071</v>
+      </c>
+      <c r="B123" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C123" s="60"/>
+      <c r="D123" s="52"/>
+      <c r="E123" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F123" s="61" t="s">
+        <v>284</v>
+      </c>
+      <c r="G123" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H123" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I123" s="50" t="n">
+        <v>122235005</v>
+      </c>
+      <c r="J123" s="50" t="s">
+        <v>285</v>
+      </c>
+      <c r="K123" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="50" t="n">
+        <v>2072</v>
+      </c>
+      <c r="B124" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C124" s="60"/>
+      <c r="D124" s="52"/>
+      <c r="E124" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F124" s="61" t="s">
+        <v>286</v>
+      </c>
+      <c r="G124" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H124" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I124" s="50" t="n">
+        <v>442759006</v>
+      </c>
+      <c r="J124" s="50" t="s">
+        <v>287</v>
+      </c>
+      <c r="K124" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="50" t="n">
+        <v>2073</v>
+      </c>
+      <c r="B125" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C125" s="60"/>
+      <c r="D125" s="52"/>
+      <c r="E125" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F125" s="61" t="s">
+        <v>288</v>
+      </c>
+      <c r="G125" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H125" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I125" s="50" t="n">
+        <v>14740000</v>
+      </c>
+      <c r="J125" s="50" t="s">
+        <v>289</v>
+      </c>
+      <c r="K125" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="50" t="n">
+        <v>2074</v>
+      </c>
+      <c r="B126" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C126" s="60"/>
+      <c r="D126" s="52"/>
+      <c r="E126" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F126" s="61" t="s">
+        <v>290</v>
+      </c>
+      <c r="G126" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H126" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I126" s="50" t="n">
+        <v>134265006</v>
+      </c>
+      <c r="J126" s="50" t="s">
+        <v>291</v>
+      </c>
+      <c r="K126" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="50" t="n">
+        <v>2075</v>
+      </c>
+      <c r="B127" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C127" s="60"/>
+      <c r="D127" s="52"/>
+      <c r="E127" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F127" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="G127" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H127" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I127" s="50" t="n">
+        <v>415121006</v>
+      </c>
+      <c r="J127" s="50" t="s">
+        <v>293</v>
+      </c>
+      <c r="K127" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="50" t="n">
+        <v>2078</v>
+      </c>
+      <c r="B130" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C130" s="60"/>
+      <c r="D130" s="52"/>
+      <c r="E130" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F130" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="G130" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H130" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I130" s="50" t="n">
+        <v>121967001</v>
+      </c>
+      <c r="J130" s="50" t="s">
+        <v>295</v>
+      </c>
+      <c r="K130" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L130" s="50"/>
+    </row>
+    <row r="131" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="50" t="n">
+        <v>2079</v>
+      </c>
+      <c r="B131" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C131" s="60"/>
+      <c r="D131" s="52"/>
+      <c r="E131" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F131" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="G131" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H131" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I131" s="50" t="n">
+        <v>88645003</v>
+      </c>
+      <c r="J131" s="50" t="s">
+        <v>297</v>
+      </c>
+      <c r="K131" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L131" s="50"/>
+    </row>
+    <row r="132" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="50" t="n">
+        <v>2080</v>
+      </c>
+      <c r="B132" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C132" s="60"/>
+      <c r="D132" s="52"/>
+      <c r="E132" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F132" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="G132" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H132" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I132" s="50" t="n">
+        <v>105050005</v>
+      </c>
+      <c r="J132" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="K132" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L132" s="50"/>
+    </row>
+    <row r="133" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="50" t="n">
+        <v>2081</v>
+      </c>
+      <c r="B133" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C133" s="60"/>
+      <c r="D133" s="52"/>
+      <c r="E133" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F133" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="G133" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H133" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I133" s="50" t="n">
+        <v>37188009</v>
+      </c>
+      <c r="J133" s="50" t="s">
+        <v>299</v>
+      </c>
+      <c r="K133" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L133" s="50"/>
+    </row>
+    <row r="134" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="50" t="n">
+        <v>2082</v>
+      </c>
+      <c r="B134" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C134" s="60"/>
+      <c r="D134" s="52"/>
+      <c r="E134" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F134" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="G134" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H134" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I134" s="50" t="n">
+        <v>105347003</v>
+      </c>
+      <c r="J134" s="50" t="s">
+        <v>301</v>
+      </c>
+      <c r="K134" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L134" s="50"/>
+    </row>
+    <row r="135" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="50" t="n">
+        <v>2083</v>
+      </c>
+      <c r="B135" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C135" s="60"/>
+      <c r="D135" s="52"/>
+      <c r="E135" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F135" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="G135" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H135" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I135" s="50" t="n">
+        <v>70979007</v>
+      </c>
+      <c r="J135" s="50" t="s">
+        <v>303</v>
+      </c>
+      <c r="K135" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L135" s="50"/>
+    </row>
+    <row r="136" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="50" t="n">
+        <v>2084</v>
+      </c>
+      <c r="B136" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C136" s="60"/>
+      <c r="D136" s="52"/>
+      <c r="E136" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F136" s="61" t="s">
+        <v>304</v>
+      </c>
+      <c r="G136" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H136" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I136" s="50" t="n">
+        <v>7932007</v>
+      </c>
+      <c r="J136" s="50" t="s">
+        <v>305</v>
+      </c>
+      <c r="K136" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L136" s="50"/>
+    </row>
+    <row r="137" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="50" t="n">
+        <v>2085</v>
+      </c>
+      <c r="B137" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C137" s="60"/>
+      <c r="D137" s="52"/>
+      <c r="E137" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F137" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="G137" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H137" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I137" s="50" t="n">
+        <v>87978006</v>
+      </c>
+      <c r="J137" s="50" t="s">
+        <v>307</v>
+      </c>
+      <c r="K137" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L137" s="50"/>
+    </row>
+    <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="50" t="n">
+        <v>2086</v>
+      </c>
+      <c r="B138" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C138" s="60"/>
+      <c r="D138" s="52"/>
+      <c r="E138" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F138" s="61" t="s">
+        <v>308</v>
+      </c>
+      <c r="G138" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H138" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I138" s="50" t="n">
+        <v>121915000</v>
+      </c>
+      <c r="J138" s="50" t="s">
+        <v>309</v>
+      </c>
+      <c r="K138" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L138" s="50"/>
+    </row>
+    <row r="139" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="50" t="n">
+        <v>2087</v>
+      </c>
+      <c r="B139" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C139" s="60"/>
+      <c r="D139" s="52"/>
+      <c r="E139" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F139" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="G139" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H139" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I139" s="50" t="n">
+        <v>315071008</v>
+      </c>
+      <c r="J139" s="50" t="s">
+        <v>311</v>
+      </c>
+      <c r="K139" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L139" s="50"/>
+    </row>
+    <row r="140" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="50" t="n">
+        <v>2088</v>
+      </c>
+      <c r="B140" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C140" s="60"/>
+      <c r="D140" s="52"/>
+      <c r="E140" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F140" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="G140" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H140" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I140" s="50" t="n">
+        <v>59960001</v>
+      </c>
+      <c r="J140" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="K140" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L140" s="50"/>
+    </row>
+    <row r="141" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="50" t="n">
+        <v>2089</v>
+      </c>
+      <c r="B141" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C141" s="60"/>
+      <c r="D141" s="52"/>
+      <c r="E141" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F141" s="61" t="s">
+        <v>312</v>
+      </c>
+      <c r="G141" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H141" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I141" s="50" t="n">
+        <v>55949003</v>
+      </c>
+      <c r="J141" s="50" t="s">
+        <v>313</v>
+      </c>
+      <c r="K141" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L141" s="50"/>
+    </row>
+    <row r="142" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="50" t="n">
+        <v>2090</v>
+      </c>
+      <c r="B142" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C142" s="60"/>
+      <c r="D142" s="52"/>
+      <c r="E142" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F142" s="61" t="s">
+        <v>314</v>
+      </c>
+      <c r="G142" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H142" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I142" s="50" t="n">
+        <v>105066007</v>
+      </c>
+      <c r="J142" s="50" t="s">
+        <v>315</v>
+      </c>
+      <c r="K142" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L142" s="50"/>
+    </row>
+    <row r="143" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="50" t="n">
+        <v>2091</v>
+      </c>
+      <c r="B143" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C143" s="60"/>
+      <c r="D143" s="52"/>
+      <c r="E143" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F143" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="G143" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H143" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I143" s="50" t="n">
+        <v>105099009</v>
+      </c>
+      <c r="J143" s="50" t="s">
+        <v>317</v>
+      </c>
+      <c r="K143" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L143" s="50"/>
+    </row>
+    <row r="144" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="50" t="n">
+        <v>2092</v>
+      </c>
+      <c r="B144" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C144" s="60"/>
+      <c r="D144" s="52"/>
+      <c r="E144" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F144" s="61" t="s">
+        <v>318</v>
+      </c>
+      <c r="G144" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H144" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I144" s="50" t="n">
+        <v>81171006</v>
+      </c>
+      <c r="J144" s="50" t="s">
+        <v>319</v>
+      </c>
+      <c r="K144" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L144" s="50"/>
+    </row>
+    <row r="145" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="50" t="n">
+        <v>2093</v>
+      </c>
+      <c r="B145" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C145" s="60"/>
+      <c r="D145" s="52"/>
+      <c r="E145" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F145" s="61" t="s">
+        <v>320</v>
+      </c>
+      <c r="G145" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H145" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I145" s="50" t="n">
+        <v>105018000</v>
+      </c>
+      <c r="J145" s="50" t="s">
+        <v>321</v>
+      </c>
+      <c r="K145" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L145" s="50"/>
+    </row>
+    <row r="146" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="50" t="n">
+        <v>2094</v>
+      </c>
+      <c r="B146" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C146" s="60"/>
+      <c r="D146" s="52"/>
+      <c r="E146" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F146" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="G146" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H146" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I146" s="50" t="n">
+        <v>49315002</v>
+      </c>
+      <c r="J146" s="50" t="s">
+        <v>323</v>
+      </c>
+      <c r="K146" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L146" s="50"/>
+    </row>
+    <row r="147" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="50" t="n">
+        <v>2095</v>
+      </c>
+      <c r="B147" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C147" s="60"/>
+      <c r="D147" s="52"/>
+      <c r="E147" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F147" s="61" t="s">
+        <v>324</v>
+      </c>
+      <c r="G147" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H147" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I147" s="50" t="n">
+        <v>104957004</v>
+      </c>
+      <c r="J147" s="50" t="s">
+        <v>325</v>
+      </c>
+      <c r="K147" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L147" s="50"/>
+    </row>
+    <row r="148" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="50" t="n">
+        <v>2096</v>
+      </c>
+      <c r="B148" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C148" s="60"/>
+      <c r="D148" s="52"/>
+      <c r="E148" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F148" s="61" t="s">
+        <v>326</v>
+      </c>
+      <c r="G148" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H148" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I148" s="50" t="n">
+        <v>105278002</v>
+      </c>
+      <c r="J148" s="50" t="s">
+        <v>327</v>
+      </c>
+      <c r="K148" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L148" s="50"/>
+    </row>
+    <row r="149" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="50" t="n">
+        <v>2097</v>
+      </c>
+      <c r="B149" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C149" s="60"/>
+      <c r="D149" s="52"/>
+      <c r="E149" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F149" s="61" t="s">
+        <v>328</v>
+      </c>
+      <c r="G149" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H149" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I149" s="50" t="n">
+        <v>105141006</v>
+      </c>
+      <c r="J149" s="50" t="s">
+        <v>329</v>
+      </c>
+      <c r="K149" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L149" s="50"/>
+    </row>
+    <row r="151" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="50" t="n">
+        <v>2099</v>
+      </c>
+      <c r="B151" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C151" s="60"/>
+      <c r="D151" s="52"/>
+      <c r="E151" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F151" s="61" t="s">
+        <v>330</v>
+      </c>
+      <c r="G151" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H151" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I151" s="50" t="n">
+        <v>121324000</v>
+      </c>
+      <c r="J151" s="50" t="s">
+        <v>331</v>
+      </c>
+      <c r="K151" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L151" s="50"/>
+    </row>
+    <row r="152" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="50" t="n">
+        <v>2100</v>
+      </c>
+      <c r="B152" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C152" s="60"/>
+      <c r="D152" s="52"/>
+      <c r="E152" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F152" s="61" t="s">
+        <v>332</v>
+      </c>
+      <c r="G152" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H152" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I152" s="50" t="n">
+        <v>16572002</v>
+      </c>
+      <c r="J152" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K152" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L152" s="50"/>
+    </row>
+    <row r="153" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="50" t="n">
+        <v>2101</v>
+      </c>
+      <c r="B153" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C153" s="60"/>
+      <c r="D153" s="52"/>
+      <c r="E153" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F153" s="61" t="s">
+        <v>334</v>
+      </c>
+      <c r="G153" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H153" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I153" s="50" t="n">
+        <v>46093004</v>
+      </c>
+      <c r="J153" s="50" t="s">
+        <v>335</v>
+      </c>
+      <c r="K153" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L153" s="50"/>
+    </row>
+    <row r="154" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="50" t="n">
+        <v>2102</v>
+      </c>
+      <c r="B154" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C154" s="60"/>
+      <c r="D154" s="52"/>
+      <c r="E154" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F154" s="61" t="s">
+        <v>336</v>
+      </c>
+      <c r="G154" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H154" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I154" s="50" t="n">
+        <v>117745003</v>
+      </c>
+      <c r="J154" s="50" t="s">
+        <v>337</v>
+      </c>
+      <c r="K154" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L154" s="50"/>
+    </row>
+    <row r="155" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="50" t="n">
+        <v>2103</v>
+      </c>
+      <c r="B155" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C155" s="60"/>
+      <c r="D155" s="52"/>
+      <c r="E155" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F155" s="61" t="s">
+        <v>338</v>
+      </c>
+      <c r="G155" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H155" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I155" s="50" t="n">
+        <v>105142004</v>
+      </c>
+      <c r="J155" s="50" t="s">
+        <v>339</v>
+      </c>
+      <c r="K155" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L155" s="50"/>
+    </row>
+    <row r="156" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="50" t="n">
+        <v>2104</v>
+      </c>
+      <c r="B156" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C156" s="60"/>
+      <c r="D156" s="52"/>
+      <c r="E156" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F156" s="61" t="s">
+        <v>340</v>
+      </c>
+      <c r="G156" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H156" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I156" s="50" t="n">
+        <v>118109009</v>
+      </c>
+      <c r="J156" s="50" t="s">
+        <v>341</v>
+      </c>
+      <c r="K156" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L156" s="50"/>
+    </row>
+    <row r="157" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="50" t="n">
+        <v>2105</v>
+      </c>
+      <c r="B157" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C157" s="60"/>
+      <c r="D157" s="52"/>
+      <c r="E157" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F157" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="G157" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H157" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I157" s="50" t="n">
+        <v>54540001</v>
+      </c>
+      <c r="J157" s="50" t="s">
+        <v>343</v>
+      </c>
+      <c r="K157" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L157" s="50"/>
+    </row>
+    <row r="158" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="50" t="n">
+        <v>2106</v>
+      </c>
+      <c r="B158" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C158" s="60"/>
+      <c r="D158" s="52"/>
+      <c r="E158" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F158" s="61" t="s">
+        <v>344</v>
+      </c>
+      <c r="G158" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H158" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I158" s="50" t="n">
+        <v>104605002</v>
+      </c>
+      <c r="J158" s="50" t="s">
+        <v>345</v>
+      </c>
+      <c r="K158" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L158" s="50"/>
+    </row>
+    <row r="159" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="50" t="n">
+        <v>2107</v>
+      </c>
+      <c r="B159" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C159" s="60"/>
+      <c r="D159" s="52"/>
+      <c r="E159" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F159" s="61" t="s">
+        <v>346</v>
+      </c>
+      <c r="G159" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H159" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I159" s="50" t="n">
+        <v>76960001</v>
+      </c>
+      <c r="J159" s="50" t="s">
+        <v>347</v>
+      </c>
+      <c r="K159" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L159" s="50"/>
+    </row>
+    <row r="160" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="50" t="n">
+        <v>2108</v>
+      </c>
+      <c r="B160" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C160" s="60"/>
+      <c r="D160" s="52"/>
+      <c r="E160" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F160" s="61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G160" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H160" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I160" s="50" t="n">
+        <v>121934000</v>
+      </c>
+      <c r="J160" s="50" t="s">
+        <v>349</v>
+      </c>
+      <c r="K160" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L160" s="50"/>
+    </row>
+    <row r="161" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="50" t="n">
+        <v>2109</v>
+      </c>
+      <c r="B161" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C161" s="60"/>
+      <c r="D161" s="52"/>
+      <c r="E161" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F161" s="61" t="s">
+        <v>350</v>
+      </c>
+      <c r="G161" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H161" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I161" s="50" t="n">
+        <v>121318006</v>
+      </c>
+      <c r="J161" s="50" t="s">
+        <v>351</v>
+      </c>
+      <c r="K161" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L161" s="50"/>
+    </row>
+    <row r="162" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="50" t="n">
+        <v>2110</v>
+      </c>
+      <c r="B162" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C162" s="60"/>
+      <c r="D162" s="52"/>
+      <c r="E162" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F162" s="61" t="s">
+        <v>352</v>
+      </c>
+      <c r="G162" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H162" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I162" s="50" t="n">
+        <v>33966007</v>
+      </c>
+      <c r="J162" s="50" t="s">
+        <v>353</v>
+      </c>
+      <c r="K162" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L162" s="50"/>
+    </row>
+    <row r="163" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="50" t="n">
+        <v>2111</v>
+      </c>
+      <c r="B163" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C163" s="60"/>
+      <c r="D163" s="52"/>
+      <c r="E163" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F163" s="61" t="s">
+        <v>354</v>
+      </c>
+      <c r="G163" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H163" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I163" s="50" t="n">
+        <v>104314002</v>
+      </c>
+      <c r="J163" s="50" t="s">
+        <v>355</v>
+      </c>
+      <c r="K163" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L163" s="50"/>
+    </row>
+    <row r="164" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="50" t="n">
+        <v>2112</v>
+      </c>
+      <c r="B164" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C164" s="60"/>
+      <c r="D164" s="52"/>
+      <c r="E164" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F164" s="61" t="s">
+        <v>356</v>
+      </c>
+      <c r="G164" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H164" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I164" s="50" t="n">
+        <v>121372004</v>
+      </c>
+      <c r="J164" s="50" t="s">
+        <v>357</v>
+      </c>
+      <c r="K164" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L164" s="50"/>
+    </row>
+    <row r="165" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="50" t="n">
+        <v>2113</v>
+      </c>
+      <c r="B165" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C165" s="60"/>
+      <c r="D165" s="52"/>
+      <c r="E165" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F165" s="61" t="s">
+        <v>358</v>
+      </c>
+      <c r="G165" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H165" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I165" s="50" t="n">
+        <v>105247001</v>
+      </c>
+      <c r="J165" s="50" t="s">
+        <v>359</v>
+      </c>
+      <c r="K165" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L165" s="50"/>
+    </row>
+    <row r="166" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="50" t="n">
+        <v>2114</v>
+      </c>
+      <c r="B166" s="60" t="n">
+        <v>42109</v>
+      </c>
+      <c r="C166" s="60"/>
+      <c r="D166" s="52"/>
+      <c r="E166" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F166" s="61" t="s">
+        <v>360</v>
+      </c>
+      <c r="G166" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H166" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I166" s="50" t="n">
+        <v>104315001</v>
+      </c>
+      <c r="J166" s="50" t="s">
+        <v>361</v>
+      </c>
+      <c r="K166" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L166" s="50"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>

</xml_diff>

<commit_message>
June rules, code updates for new RxNorm format
</commit_message>
<xml_diff>
--- a/db-processing-rules/src/main/resources/SOLOR LOINC Rules.xlsx
+++ b/db-processing-rules/src/main/resources/SOLOR LOINC Rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="638" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="526" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="446">
   <si>
     <t>ID</t>
   </si>
@@ -1102,16 +1102,267 @@
   </si>
   <si>
     <t>measurement of Western equine encephalitis virus antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Immune complex</t>
+  </si>
+  <si>
+    <t>immune complex assay (procedure)</t>
+  </si>
+  <si>
+    <t>Epstein Barr virus DNA</t>
+  </si>
+  <si>
+    <t>Epstein Barr virus deoxyribonucleic acid assay (procedure)</t>
+  </si>
+  <si>
+    <t>Manganese</t>
+  </si>
+  <si>
+    <t>manganese measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Carnitine</t>
+  </si>
+  <si>
+    <t>carnitine measurement (procedure)</t>
+  </si>
+  <si>
+    <t>La Crosse virus Ab</t>
+  </si>
+  <si>
+    <t>measurement of La Crosse virus antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Methanol</t>
+  </si>
+  <si>
+    <t>alcohol, methyl measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Hydroxyethylflurazepam</t>
+  </si>
+  <si>
+    <t>hydroxyethylflurazepam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Hydroxyproline</t>
+  </si>
+  <si>
+    <t>hydroxyproline measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Thallium</t>
+  </si>
+  <si>
+    <t>thallium measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Specific gravity</t>
+  </si>
+  <si>
+    <t>specific gravity measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Beta-2-Microglobulin</t>
+  </si>
+  <si>
+    <t>Beta-2-microglobulin measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Antimony</t>
+  </si>
+  <si>
+    <t>antimony measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Influenza virus A Ag</t>
+  </si>
+  <si>
+    <t>Influenza virus A antigen assay (procedure)</t>
+  </si>
+  <si>
+    <t>Hydroxytriazolam</t>
+  </si>
+  <si>
+    <t>hydroxytriazolam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Butabarbital</t>
+  </si>
+  <si>
+    <t>butabarbital measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Bismuth</t>
+  </si>
+  <si>
+    <t>bismuth measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Clobazam</t>
+  </si>
+  <si>
+    <t>clobazam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Cocaethylene</t>
+  </si>
+  <si>
+    <t>cocaethylene measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>silver measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Molybdenum</t>
+  </si>
+  <si>
+    <t>molybdenum measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Cytomegalovirus Ab</t>
+  </si>
+  <si>
+    <t>serologic test for cytomegalovirus (procedure)</t>
+  </si>
+  <si>
+    <t>Influenza virus B Ag</t>
+  </si>
+  <si>
+    <t>Influenza virus B antigen assay (procedure)</t>
+  </si>
+  <si>
+    <t>Lithium</t>
+  </si>
+  <si>
+    <t>lithium measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Hydromorphone</t>
+  </si>
+  <si>
+    <t>hydromorphone measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Herpes simplex virus 2 Ab.IgM</t>
+  </si>
+  <si>
+    <t>measurement of Human herpesvirus 2 antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Alpha-1-Fetoprotein</t>
+  </si>
+  <si>
+    <t>alpha-1-Fetoprotein measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Chlamydia trachomatis DNA</t>
+  </si>
+  <si>
+    <t>Chlamydia trachomatis deoxyribonucleic acid assay (procedure)</t>
+  </si>
+  <si>
+    <t>Fentanyl</t>
+  </si>
+  <si>
+    <t>fentanyl measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Salicylates</t>
+  </si>
+  <si>
+    <t>salicylate measurement (procedure)</t>
+  </si>
+  <si>
+    <t>West Nile virus Ab.IgM</t>
+  </si>
+  <si>
+    <t>West Nile virus immunoglobulin M antibody measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Methylenedioxymethamphetamine</t>
+  </si>
+  <si>
+    <t>methylenedioxymethamphetamine measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Rabies virus Ab</t>
+  </si>
+  <si>
+    <t>measurement of Rabies virus antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Strychnine</t>
+  </si>
+  <si>
+    <t>strychnine measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Isopropanol</t>
+  </si>
+  <si>
+    <t>isopropanol measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Aspergillus sp Ab</t>
+  </si>
+  <si>
+    <t>serologic test for Aspergillus (procedure)</t>
+  </si>
+  <si>
+    <t>Hydrocodone</t>
+  </si>
+  <si>
+    <t>Hydrocodone measurement (procedure)</t>
+  </si>
+  <si>
+    <t>La Crosse virus Ab.IgM</t>
+  </si>
+  <si>
+    <t>Herpes simplex virus 2 Ab</t>
+  </si>
+  <si>
+    <t>Histoplasma capsulatum Ab</t>
+  </si>
+  <si>
+    <t>measurement of Histoplasma capsulatum antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Adenovirus Ab</t>
+  </si>
+  <si>
+    <t>measurement of adenovirus antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Measles virus Ab.IgG</t>
+  </si>
+  <si>
+    <t>measurement of Measles virus antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Estradiol</t>
+  </si>
+  <si>
+    <t>estradiol measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Cortisol</t>
+  </si>
+  <si>
+    <t>cortisol measurement (procedure)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="D\-MMM\-YY;@"/>
-    <numFmt numFmtId="166" formatCode="D\-MMM\-YY;@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -1137,13 +1388,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1151,8 +1395,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1181,6 +1432,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF993366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF767171"/>
+        <bgColor rgb="FF7C7C7C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7C7C7C"/>
+        <bgColor rgb="FF767171"/>
       </patternFill>
     </fill>
   </fills>
@@ -1308,25 +1571,25 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="71">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1334,7 +1597,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1350,19 +1613,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1538,7 +1801,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1546,27 +1809,63 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1578,9 +1877,9 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Normal_LOINC Rules" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Normal_LOINC Rules" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Normal_LOINC Rules" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Normal 2" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Normal_LOINC Rules" xfId="22" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1599,7 +1898,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC5E0B4"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF7C7C7C"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF7030A0"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -1630,7 +1929,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF767171"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -1767,10 +2066,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BB166"/>
+  <dimension ref="A1:BB223"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A167" activeCellId="0" sqref="A167"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A187" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B168" activeCellId="0" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7267,15 +7566,15 @@
       <c r="A103" s="50" t="n">
         <v>2051</v>
       </c>
-      <c r="B103" s="60" t="n">
+      <c r="B103" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C103" s="60"/>
+      <c r="C103" s="51"/>
       <c r="D103" s="52"/>
       <c r="E103" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F103" s="61" t="s">
+      <c r="F103" s="60" t="s">
         <v>247</v>
       </c>
       <c r="G103" s="50" t="s">
@@ -7298,15 +7597,15 @@
       <c r="A104" s="50" t="n">
         <v>2052</v>
       </c>
-      <c r="B104" s="60" t="n">
+      <c r="B104" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C104" s="60"/>
+      <c r="C104" s="51"/>
       <c r="D104" s="52"/>
       <c r="E104" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F104" s="61" t="s">
+      <c r="F104" s="60" t="s">
         <v>249</v>
       </c>
       <c r="G104" s="50" t="s">
@@ -7329,15 +7628,15 @@
       <c r="A105" s="50" t="n">
         <v>2053</v>
       </c>
-      <c r="B105" s="60" t="n">
+      <c r="B105" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C105" s="60"/>
+      <c r="C105" s="51"/>
       <c r="D105" s="52"/>
       <c r="E105" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F105" s="61" t="s">
+      <c r="F105" s="60" t="s">
         <v>251</v>
       </c>
       <c r="G105" s="50" t="s">
@@ -7360,15 +7659,15 @@
       <c r="A106" s="50" t="n">
         <v>2054</v>
       </c>
-      <c r="B106" s="60" t="n">
+      <c r="B106" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C106" s="60"/>
+      <c r="C106" s="51"/>
       <c r="D106" s="52"/>
       <c r="E106" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F106" s="61" t="s">
+      <c r="F106" s="60" t="s">
         <v>253</v>
       </c>
       <c r="G106" s="50" t="s">
@@ -7391,15 +7690,15 @@
       <c r="A107" s="50" t="n">
         <v>2055</v>
       </c>
-      <c r="B107" s="60" t="n">
+      <c r="B107" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C107" s="60"/>
+      <c r="C107" s="51"/>
       <c r="D107" s="52"/>
       <c r="E107" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F107" s="61" t="s">
+      <c r="F107" s="60" t="s">
         <v>255</v>
       </c>
       <c r="G107" s="50" t="s">
@@ -7422,15 +7721,15 @@
       <c r="A108" s="50" t="n">
         <v>2056</v>
       </c>
-      <c r="B108" s="60" t="n">
+      <c r="B108" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C108" s="60"/>
+      <c r="C108" s="51"/>
       <c r="D108" s="52"/>
       <c r="E108" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F108" s="61" t="s">
+      <c r="F108" s="60" t="s">
         <v>256</v>
       </c>
       <c r="G108" s="50" t="s">
@@ -7453,15 +7752,15 @@
       <c r="A109" s="50" t="n">
         <v>2057</v>
       </c>
-      <c r="B109" s="60" t="n">
+      <c r="B109" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C109" s="60"/>
+      <c r="C109" s="51"/>
       <c r="D109" s="52"/>
       <c r="E109" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F109" s="61" t="s">
+      <c r="F109" s="60" t="s">
         <v>258</v>
       </c>
       <c r="G109" s="50" t="s">
@@ -7484,15 +7783,15 @@
       <c r="A110" s="50" t="n">
         <v>2058</v>
       </c>
-      <c r="B110" s="60" t="n">
+      <c r="B110" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C110" s="60"/>
+      <c r="C110" s="51"/>
       <c r="D110" s="52"/>
       <c r="E110" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F110" s="61" t="s">
+      <c r="F110" s="60" t="s">
         <v>260</v>
       </c>
       <c r="G110" s="50" t="s">
@@ -7515,15 +7814,15 @@
       <c r="A111" s="50" t="n">
         <v>2059</v>
       </c>
-      <c r="B111" s="60" t="n">
+      <c r="B111" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C111" s="60"/>
+      <c r="C111" s="51"/>
       <c r="D111" s="52"/>
       <c r="E111" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F111" s="61" t="s">
+      <c r="F111" s="60" t="s">
         <v>262</v>
       </c>
       <c r="G111" s="50" t="s">
@@ -7546,15 +7845,15 @@
       <c r="A112" s="50" t="n">
         <v>2060</v>
       </c>
-      <c r="B112" s="60" t="n">
+      <c r="B112" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C112" s="60"/>
+      <c r="C112" s="51"/>
       <c r="D112" s="52"/>
       <c r="E112" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F112" s="61" t="s">
+      <c r="F112" s="60" t="s">
         <v>264</v>
       </c>
       <c r="G112" s="50" t="s">
@@ -7577,15 +7876,15 @@
       <c r="A113" s="50" t="n">
         <v>2061</v>
       </c>
-      <c r="B113" s="60" t="n">
+      <c r="B113" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C113" s="60"/>
+      <c r="C113" s="51"/>
       <c r="D113" s="52"/>
       <c r="E113" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F113" s="61" t="s">
+      <c r="F113" s="60" t="s">
         <v>266</v>
       </c>
       <c r="G113" s="50" t="s">
@@ -7608,15 +7907,15 @@
       <c r="A114" s="50" t="n">
         <v>2062</v>
       </c>
-      <c r="B114" s="60" t="n">
+      <c r="B114" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C114" s="60"/>
+      <c r="C114" s="51"/>
       <c r="D114" s="52"/>
       <c r="E114" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F114" s="61" t="s">
+      <c r="F114" s="60" t="s">
         <v>268</v>
       </c>
       <c r="G114" s="50" t="s">
@@ -7639,15 +7938,15 @@
       <c r="A115" s="50" t="n">
         <v>2063</v>
       </c>
-      <c r="B115" s="60" t="n">
+      <c r="B115" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C115" s="60"/>
+      <c r="C115" s="51"/>
       <c r="D115" s="52"/>
       <c r="E115" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F115" s="61" t="s">
+      <c r="F115" s="60" t="s">
         <v>270</v>
       </c>
       <c r="G115" s="50" t="s">
@@ -7670,15 +7969,15 @@
       <c r="A116" s="50" t="n">
         <v>2064</v>
       </c>
-      <c r="B116" s="60" t="n">
+      <c r="B116" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C116" s="60"/>
+      <c r="C116" s="51"/>
       <c r="D116" s="52"/>
       <c r="E116" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F116" s="61" t="s">
+      <c r="F116" s="60" t="s">
         <v>272</v>
       </c>
       <c r="G116" s="50" t="s">
@@ -7701,15 +8000,15 @@
       <c r="A117" s="50" t="n">
         <v>2065</v>
       </c>
-      <c r="B117" s="60" t="n">
+      <c r="B117" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C117" s="60"/>
+      <c r="C117" s="51"/>
       <c r="D117" s="52"/>
       <c r="E117" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F117" s="61" t="s">
+      <c r="F117" s="60" t="s">
         <v>274</v>
       </c>
       <c r="G117" s="50" t="s">
@@ -7732,15 +8031,15 @@
       <c r="A118" s="50" t="n">
         <v>2066</v>
       </c>
-      <c r="B118" s="60" t="n">
+      <c r="B118" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C118" s="60"/>
+      <c r="C118" s="51"/>
       <c r="D118" s="52"/>
       <c r="E118" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F118" s="61" t="s">
+      <c r="F118" s="60" t="s">
         <v>276</v>
       </c>
       <c r="G118" s="50" t="s">
@@ -7763,15 +8062,15 @@
       <c r="A119" s="50" t="n">
         <v>2067</v>
       </c>
-      <c r="B119" s="60" t="n">
+      <c r="B119" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C119" s="60"/>
+      <c r="C119" s="51"/>
       <c r="D119" s="52"/>
       <c r="E119" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F119" s="61" t="s">
+      <c r="F119" s="60" t="s">
         <v>74</v>
       </c>
       <c r="G119" s="50" t="s">
@@ -7794,15 +8093,15 @@
       <c r="A120" s="50" t="n">
         <v>2068</v>
       </c>
-      <c r="B120" s="60" t="n">
+      <c r="B120" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C120" s="60"/>
+      <c r="C120" s="51"/>
       <c r="D120" s="52"/>
       <c r="E120" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F120" s="61" t="s">
+      <c r="F120" s="60" t="s">
         <v>278</v>
       </c>
       <c r="G120" s="50" t="s">
@@ -7825,15 +8124,15 @@
       <c r="A121" s="50" t="n">
         <v>2069</v>
       </c>
-      <c r="B121" s="60" t="n">
+      <c r="B121" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C121" s="60"/>
+      <c r="C121" s="51"/>
       <c r="D121" s="52"/>
       <c r="E121" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F121" s="61" t="s">
+      <c r="F121" s="60" t="s">
         <v>280</v>
       </c>
       <c r="G121" s="50" t="s">
@@ -7856,15 +8155,15 @@
       <c r="A122" s="50" t="n">
         <v>2070</v>
       </c>
-      <c r="B122" s="60" t="n">
+      <c r="B122" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C122" s="60"/>
+      <c r="C122" s="51"/>
       <c r="D122" s="52"/>
       <c r="E122" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F122" s="61" t="s">
+      <c r="F122" s="60" t="s">
         <v>282</v>
       </c>
       <c r="G122" s="50" t="s">
@@ -7887,15 +8186,15 @@
       <c r="A123" s="50" t="n">
         <v>2071</v>
       </c>
-      <c r="B123" s="60" t="n">
+      <c r="B123" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C123" s="60"/>
+      <c r="C123" s="51"/>
       <c r="D123" s="52"/>
       <c r="E123" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F123" s="61" t="s">
+      <c r="F123" s="60" t="s">
         <v>284</v>
       </c>
       <c r="G123" s="50" t="s">
@@ -7918,15 +8217,15 @@
       <c r="A124" s="50" t="n">
         <v>2072</v>
       </c>
-      <c r="B124" s="60" t="n">
+      <c r="B124" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C124" s="60"/>
+      <c r="C124" s="51"/>
       <c r="D124" s="52"/>
       <c r="E124" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F124" s="61" t="s">
+      <c r="F124" s="60" t="s">
         <v>286</v>
       </c>
       <c r="G124" s="50" t="s">
@@ -7949,15 +8248,15 @@
       <c r="A125" s="50" t="n">
         <v>2073</v>
       </c>
-      <c r="B125" s="60" t="n">
+      <c r="B125" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C125" s="60"/>
+      <c r="C125" s="51"/>
       <c r="D125" s="52"/>
       <c r="E125" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F125" s="61" t="s">
+      <c r="F125" s="60" t="s">
         <v>288</v>
       </c>
       <c r="G125" s="50" t="s">
@@ -7980,15 +8279,15 @@
       <c r="A126" s="50" t="n">
         <v>2074</v>
       </c>
-      <c r="B126" s="60" t="n">
+      <c r="B126" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C126" s="60"/>
+      <c r="C126" s="51"/>
       <c r="D126" s="52"/>
       <c r="E126" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F126" s="61" t="s">
+      <c r="F126" s="60" t="s">
         <v>290</v>
       </c>
       <c r="G126" s="50" t="s">
@@ -8011,15 +8310,15 @@
       <c r="A127" s="50" t="n">
         <v>2075</v>
       </c>
-      <c r="B127" s="60" t="n">
+      <c r="B127" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C127" s="60"/>
+      <c r="C127" s="51"/>
       <c r="D127" s="52"/>
       <c r="E127" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F127" s="61" t="s">
+      <c r="F127" s="60" t="s">
         <v>292</v>
       </c>
       <c r="G127" s="50" t="s">
@@ -8037,20 +8336,26 @@
       <c r="K127" s="50" t="s">
         <v>28</v>
       </c>
+    </row>
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D128" s="0"/>
+    </row>
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D129" s="0"/>
     </row>
     <row r="130" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="50" t="n">
         <v>2078</v>
       </c>
-      <c r="B130" s="60" t="n">
+      <c r="B130" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C130" s="60"/>
+      <c r="C130" s="51"/>
       <c r="D130" s="52"/>
       <c r="E130" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F130" s="61" t="s">
+      <c r="F130" s="60" t="s">
         <v>294</v>
       </c>
       <c r="G130" s="50" t="s">
@@ -8074,15 +8379,15 @@
       <c r="A131" s="50" t="n">
         <v>2079</v>
       </c>
-      <c r="B131" s="60" t="n">
+      <c r="B131" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C131" s="60"/>
+      <c r="C131" s="51"/>
       <c r="D131" s="52"/>
       <c r="E131" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F131" s="61" t="s">
+      <c r="F131" s="60" t="s">
         <v>296</v>
       </c>
       <c r="G131" s="50" t="s">
@@ -8106,15 +8411,15 @@
       <c r="A132" s="50" t="n">
         <v>2080</v>
       </c>
-      <c r="B132" s="60" t="n">
+      <c r="B132" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C132" s="60"/>
+      <c r="C132" s="51"/>
       <c r="D132" s="52"/>
       <c r="E132" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F132" s="61" t="s">
+      <c r="F132" s="60" t="s">
         <v>97</v>
       </c>
       <c r="G132" s="50" t="s">
@@ -8138,15 +8443,15 @@
       <c r="A133" s="50" t="n">
         <v>2081</v>
       </c>
-      <c r="B133" s="60" t="n">
+      <c r="B133" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C133" s="60"/>
+      <c r="C133" s="51"/>
       <c r="D133" s="52"/>
       <c r="E133" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F133" s="61" t="s">
+      <c r="F133" s="60" t="s">
         <v>298</v>
       </c>
       <c r="G133" s="50" t="s">
@@ -8170,15 +8475,15 @@
       <c r="A134" s="50" t="n">
         <v>2082</v>
       </c>
-      <c r="B134" s="60" t="n">
+      <c r="B134" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C134" s="60"/>
+      <c r="C134" s="51"/>
       <c r="D134" s="52"/>
       <c r="E134" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F134" s="61" t="s">
+      <c r="F134" s="60" t="s">
         <v>300</v>
       </c>
       <c r="G134" s="50" t="s">
@@ -8202,15 +8507,15 @@
       <c r="A135" s="50" t="n">
         <v>2083</v>
       </c>
-      <c r="B135" s="60" t="n">
+      <c r="B135" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C135" s="60"/>
+      <c r="C135" s="51"/>
       <c r="D135" s="52"/>
       <c r="E135" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F135" s="61" t="s">
+      <c r="F135" s="60" t="s">
         <v>302</v>
       </c>
       <c r="G135" s="50" t="s">
@@ -8234,15 +8539,15 @@
       <c r="A136" s="50" t="n">
         <v>2084</v>
       </c>
-      <c r="B136" s="60" t="n">
+      <c r="B136" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C136" s="60"/>
+      <c r="C136" s="51"/>
       <c r="D136" s="52"/>
       <c r="E136" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F136" s="61" t="s">
+      <c r="F136" s="60" t="s">
         <v>304</v>
       </c>
       <c r="G136" s="50" t="s">
@@ -8266,15 +8571,15 @@
       <c r="A137" s="50" t="n">
         <v>2085</v>
       </c>
-      <c r="B137" s="60" t="n">
+      <c r="B137" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C137" s="60"/>
+      <c r="C137" s="51"/>
       <c r="D137" s="52"/>
       <c r="E137" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F137" s="61" t="s">
+      <c r="F137" s="60" t="s">
         <v>306</v>
       </c>
       <c r="G137" s="50" t="s">
@@ -8298,15 +8603,15 @@
       <c r="A138" s="50" t="n">
         <v>2086</v>
       </c>
-      <c r="B138" s="60" t="n">
+      <c r="B138" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C138" s="60"/>
+      <c r="C138" s="51"/>
       <c r="D138" s="52"/>
       <c r="E138" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F138" s="61" t="s">
+      <c r="F138" s="60" t="s">
         <v>308</v>
       </c>
       <c r="G138" s="50" t="s">
@@ -8330,15 +8635,15 @@
       <c r="A139" s="50" t="n">
         <v>2087</v>
       </c>
-      <c r="B139" s="60" t="n">
+      <c r="B139" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C139" s="60"/>
+      <c r="C139" s="51"/>
       <c r="D139" s="52"/>
       <c r="E139" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F139" s="61" t="s">
+      <c r="F139" s="60" t="s">
         <v>310</v>
       </c>
       <c r="G139" s="50" t="s">
@@ -8362,15 +8667,15 @@
       <c r="A140" s="50" t="n">
         <v>2088</v>
       </c>
-      <c r="B140" s="60" t="n">
+      <c r="B140" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C140" s="60"/>
+      <c r="C140" s="51"/>
       <c r="D140" s="52"/>
       <c r="E140" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F140" s="61" t="s">
+      <c r="F140" s="60" t="s">
         <v>100</v>
       </c>
       <c r="G140" s="50" t="s">
@@ -8394,15 +8699,15 @@
       <c r="A141" s="50" t="n">
         <v>2089</v>
       </c>
-      <c r="B141" s="60" t="n">
+      <c r="B141" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C141" s="60"/>
+      <c r="C141" s="51"/>
       <c r="D141" s="52"/>
       <c r="E141" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F141" s="61" t="s">
+      <c r="F141" s="60" t="s">
         <v>312</v>
       </c>
       <c r="G141" s="50" t="s">
@@ -8426,15 +8731,15 @@
       <c r="A142" s="50" t="n">
         <v>2090</v>
       </c>
-      <c r="B142" s="60" t="n">
+      <c r="B142" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C142" s="60"/>
+      <c r="C142" s="51"/>
       <c r="D142" s="52"/>
       <c r="E142" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F142" s="61" t="s">
+      <c r="F142" s="60" t="s">
         <v>314</v>
       </c>
       <c r="G142" s="50" t="s">
@@ -8458,15 +8763,15 @@
       <c r="A143" s="50" t="n">
         <v>2091</v>
       </c>
-      <c r="B143" s="60" t="n">
+      <c r="B143" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C143" s="60"/>
+      <c r="C143" s="51"/>
       <c r="D143" s="52"/>
       <c r="E143" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F143" s="61" t="s">
+      <c r="F143" s="60" t="s">
         <v>316</v>
       </c>
       <c r="G143" s="50" t="s">
@@ -8490,15 +8795,15 @@
       <c r="A144" s="50" t="n">
         <v>2092</v>
       </c>
-      <c r="B144" s="60" t="n">
+      <c r="B144" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C144" s="60"/>
+      <c r="C144" s="51"/>
       <c r="D144" s="52"/>
       <c r="E144" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F144" s="61" t="s">
+      <c r="F144" s="60" t="s">
         <v>318</v>
       </c>
       <c r="G144" s="50" t="s">
@@ -8522,15 +8827,15 @@
       <c r="A145" s="50" t="n">
         <v>2093</v>
       </c>
-      <c r="B145" s="60" t="n">
+      <c r="B145" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C145" s="60"/>
+      <c r="C145" s="51"/>
       <c r="D145" s="52"/>
       <c r="E145" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F145" s="61" t="s">
+      <c r="F145" s="60" t="s">
         <v>320</v>
       </c>
       <c r="G145" s="50" t="s">
@@ -8554,15 +8859,15 @@
       <c r="A146" s="50" t="n">
         <v>2094</v>
       </c>
-      <c r="B146" s="60" t="n">
+      <c r="B146" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C146" s="60"/>
+      <c r="C146" s="51"/>
       <c r="D146" s="52"/>
       <c r="E146" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F146" s="61" t="s">
+      <c r="F146" s="60" t="s">
         <v>322</v>
       </c>
       <c r="G146" s="50" t="s">
@@ -8586,15 +8891,15 @@
       <c r="A147" s="50" t="n">
         <v>2095</v>
       </c>
-      <c r="B147" s="60" t="n">
+      <c r="B147" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C147" s="60"/>
+      <c r="C147" s="51"/>
       <c r="D147" s="52"/>
       <c r="E147" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F147" s="61" t="s">
+      <c r="F147" s="60" t="s">
         <v>324</v>
       </c>
       <c r="G147" s="50" t="s">
@@ -8618,15 +8923,15 @@
       <c r="A148" s="50" t="n">
         <v>2096</v>
       </c>
-      <c r="B148" s="60" t="n">
+      <c r="B148" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C148" s="60"/>
+      <c r="C148" s="51"/>
       <c r="D148" s="52"/>
       <c r="E148" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F148" s="61" t="s">
+      <c r="F148" s="60" t="s">
         <v>326</v>
       </c>
       <c r="G148" s="50" t="s">
@@ -8650,15 +8955,15 @@
       <c r="A149" s="50" t="n">
         <v>2097</v>
       </c>
-      <c r="B149" s="60" t="n">
+      <c r="B149" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C149" s="60"/>
+      <c r="C149" s="51"/>
       <c r="D149" s="52"/>
       <c r="E149" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F149" s="61" t="s">
+      <c r="F149" s="60" t="s">
         <v>328</v>
       </c>
       <c r="G149" s="50" t="s">
@@ -8677,20 +8982,23 @@
         <v>28</v>
       </c>
       <c r="L149" s="50"/>
+    </row>
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D150" s="0"/>
     </row>
     <row r="151" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="50" t="n">
         <v>2099</v>
       </c>
-      <c r="B151" s="60" t="n">
+      <c r="B151" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C151" s="60"/>
+      <c r="C151" s="51"/>
       <c r="D151" s="52"/>
       <c r="E151" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F151" s="61" t="s">
+      <c r="F151" s="60" t="s">
         <v>330</v>
       </c>
       <c r="G151" s="50" t="s">
@@ -8714,15 +9022,15 @@
       <c r="A152" s="50" t="n">
         <v>2100</v>
       </c>
-      <c r="B152" s="60" t="n">
+      <c r="B152" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C152" s="60"/>
+      <c r="C152" s="51"/>
       <c r="D152" s="52"/>
       <c r="E152" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F152" s="61" t="s">
+      <c r="F152" s="60" t="s">
         <v>332</v>
       </c>
       <c r="G152" s="50" t="s">
@@ -8746,15 +9054,15 @@
       <c r="A153" s="50" t="n">
         <v>2101</v>
       </c>
-      <c r="B153" s="60" t="n">
+      <c r="B153" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C153" s="60"/>
+      <c r="C153" s="51"/>
       <c r="D153" s="52"/>
       <c r="E153" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F153" s="61" t="s">
+      <c r="F153" s="60" t="s">
         <v>334</v>
       </c>
       <c r="G153" s="50" t="s">
@@ -8778,15 +9086,15 @@
       <c r="A154" s="50" t="n">
         <v>2102</v>
       </c>
-      <c r="B154" s="60" t="n">
+      <c r="B154" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C154" s="60"/>
+      <c r="C154" s="51"/>
       <c r="D154" s="52"/>
       <c r="E154" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F154" s="61" t="s">
+      <c r="F154" s="60" t="s">
         <v>336</v>
       </c>
       <c r="G154" s="50" t="s">
@@ -8810,15 +9118,15 @@
       <c r="A155" s="50" t="n">
         <v>2103</v>
       </c>
-      <c r="B155" s="60" t="n">
+      <c r="B155" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C155" s="60"/>
+      <c r="C155" s="51"/>
       <c r="D155" s="52"/>
       <c r="E155" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F155" s="61" t="s">
+      <c r="F155" s="60" t="s">
         <v>338</v>
       </c>
       <c r="G155" s="50" t="s">
@@ -8842,15 +9150,15 @@
       <c r="A156" s="50" t="n">
         <v>2104</v>
       </c>
-      <c r="B156" s="60" t="n">
+      <c r="B156" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C156" s="60"/>
+      <c r="C156" s="51"/>
       <c r="D156" s="52"/>
       <c r="E156" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F156" s="61" t="s">
+      <c r="F156" s="60" t="s">
         <v>340</v>
       </c>
       <c r="G156" s="50" t="s">
@@ -8874,15 +9182,15 @@
       <c r="A157" s="50" t="n">
         <v>2105</v>
       </c>
-      <c r="B157" s="60" t="n">
+      <c r="B157" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C157" s="60"/>
+      <c r="C157" s="51"/>
       <c r="D157" s="52"/>
       <c r="E157" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F157" s="61" t="s">
+      <c r="F157" s="60" t="s">
         <v>342</v>
       </c>
       <c r="G157" s="50" t="s">
@@ -8906,15 +9214,15 @@
       <c r="A158" s="50" t="n">
         <v>2106</v>
       </c>
-      <c r="B158" s="60" t="n">
+      <c r="B158" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C158" s="60"/>
+      <c r="C158" s="51"/>
       <c r="D158" s="52"/>
       <c r="E158" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F158" s="61" t="s">
+      <c r="F158" s="60" t="s">
         <v>344</v>
       </c>
       <c r="G158" s="50" t="s">
@@ -8938,15 +9246,15 @@
       <c r="A159" s="50" t="n">
         <v>2107</v>
       </c>
-      <c r="B159" s="60" t="n">
+      <c r="B159" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C159" s="60"/>
+      <c r="C159" s="51"/>
       <c r="D159" s="52"/>
       <c r="E159" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F159" s="61" t="s">
+      <c r="F159" s="60" t="s">
         <v>346</v>
       </c>
       <c r="G159" s="50" t="s">
@@ -8970,15 +9278,15 @@
       <c r="A160" s="50" t="n">
         <v>2108</v>
       </c>
-      <c r="B160" s="60" t="n">
+      <c r="B160" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C160" s="60"/>
+      <c r="C160" s="51"/>
       <c r="D160" s="52"/>
       <c r="E160" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F160" s="61" t="s">
+      <c r="F160" s="60" t="s">
         <v>348</v>
       </c>
       <c r="G160" s="50" t="s">
@@ -9002,15 +9310,15 @@
       <c r="A161" s="50" t="n">
         <v>2109</v>
       </c>
-      <c r="B161" s="60" t="n">
+      <c r="B161" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C161" s="60"/>
+      <c r="C161" s="51"/>
       <c r="D161" s="52"/>
       <c r="E161" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F161" s="61" t="s">
+      <c r="F161" s="60" t="s">
         <v>350</v>
       </c>
       <c r="G161" s="50" t="s">
@@ -9034,15 +9342,15 @@
       <c r="A162" s="50" t="n">
         <v>2110</v>
       </c>
-      <c r="B162" s="60" t="n">
+      <c r="B162" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C162" s="60"/>
+      <c r="C162" s="51"/>
       <c r="D162" s="52"/>
       <c r="E162" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F162" s="61" t="s">
+      <c r="F162" s="60" t="s">
         <v>352</v>
       </c>
       <c r="G162" s="50" t="s">
@@ -9066,15 +9374,15 @@
       <c r="A163" s="50" t="n">
         <v>2111</v>
       </c>
-      <c r="B163" s="60" t="n">
+      <c r="B163" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C163" s="60"/>
+      <c r="C163" s="51"/>
       <c r="D163" s="52"/>
       <c r="E163" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F163" s="61" t="s">
+      <c r="F163" s="60" t="s">
         <v>354</v>
       </c>
       <c r="G163" s="50" t="s">
@@ -9098,15 +9406,15 @@
       <c r="A164" s="50" t="n">
         <v>2112</v>
       </c>
-      <c r="B164" s="60" t="n">
+      <c r="B164" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C164" s="60"/>
+      <c r="C164" s="51"/>
       <c r="D164" s="52"/>
       <c r="E164" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F164" s="61" t="s">
+      <c r="F164" s="60" t="s">
         <v>356</v>
       </c>
       <c r="G164" s="50" t="s">
@@ -9130,15 +9438,15 @@
       <c r="A165" s="50" t="n">
         <v>2113</v>
       </c>
-      <c r="B165" s="60" t="n">
+      <c r="B165" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C165" s="60"/>
+      <c r="C165" s="51"/>
       <c r="D165" s="52"/>
       <c r="E165" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F165" s="61" t="s">
+      <c r="F165" s="60" t="s">
         <v>358</v>
       </c>
       <c r="G165" s="50" t="s">
@@ -9162,15 +9470,15 @@
       <c r="A166" s="50" t="n">
         <v>2114</v>
       </c>
-      <c r="B166" s="60" t="n">
+      <c r="B166" s="51" t="n">
         <v>42109</v>
       </c>
-      <c r="C166" s="60"/>
+      <c r="C166" s="51"/>
       <c r="D166" s="52"/>
       <c r="E166" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F166" s="61" t="s">
+      <c r="F166" s="60" t="s">
         <v>360</v>
       </c>
       <c r="G166" s="50" t="s">
@@ -9189,6 +9497,1578 @@
         <v>28</v>
       </c>
       <c r="L166" s="50"/>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="45"/>
+      <c r="B167" s="46"/>
+      <c r="C167" s="46"/>
+      <c r="D167" s="47"/>
+      <c r="E167" s="45"/>
+      <c r="F167" s="61"/>
+      <c r="G167" s="45"/>
+      <c r="H167" s="45"/>
+      <c r="I167" s="45"/>
+      <c r="J167" s="45"/>
+      <c r="K167" s="45"/>
+      <c r="L167" s="45"/>
+    </row>
+    <row r="168" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="50" t="n">
+        <v>2115</v>
+      </c>
+      <c r="B168" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C168" s="51"/>
+      <c r="D168" s="52"/>
+      <c r="E168" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F168" s="60" t="s">
+        <v>362</v>
+      </c>
+      <c r="G168" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H168" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I168" s="50" t="n">
+        <v>113055007</v>
+      </c>
+      <c r="J168" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="K168" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L168" s="50"/>
+    </row>
+    <row r="169" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="50" t="n">
+        <v>2116</v>
+      </c>
+      <c r="B169" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C169" s="51"/>
+      <c r="D169" s="52"/>
+      <c r="E169" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F169" s="60" t="s">
+        <v>364</v>
+      </c>
+      <c r="G169" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H169" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I169" s="50" t="n">
+        <v>122330002</v>
+      </c>
+      <c r="J169" s="50" t="s">
+        <v>365</v>
+      </c>
+      <c r="K169" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L169" s="50"/>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="62"/>
+      <c r="B170" s="63"/>
+      <c r="C170" s="63"/>
+      <c r="D170" s="64"/>
+      <c r="E170" s="62"/>
+      <c r="F170" s="65"/>
+      <c r="G170" s="62"/>
+      <c r="H170" s="62"/>
+      <c r="I170" s="62"/>
+      <c r="J170" s="62"/>
+      <c r="K170" s="62"/>
+      <c r="L170" s="62"/>
+    </row>
+    <row r="171" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="50" t="n">
+        <v>2118</v>
+      </c>
+      <c r="B171" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C171" s="51"/>
+      <c r="D171" s="52"/>
+      <c r="E171" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F171" s="60" t="s">
+        <v>366</v>
+      </c>
+      <c r="G171" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H171" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I171" s="50" t="n">
+        <v>26052003</v>
+      </c>
+      <c r="J171" s="50" t="s">
+        <v>367</v>
+      </c>
+      <c r="K171" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L171" s="50"/>
+    </row>
+    <row r="172" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="50" t="n">
+        <v>2119</v>
+      </c>
+      <c r="B172" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C172" s="51"/>
+      <c r="D172" s="52"/>
+      <c r="E172" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F172" s="60" t="s">
+        <v>368</v>
+      </c>
+      <c r="G172" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H172" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I172" s="50" t="n">
+        <v>36174000</v>
+      </c>
+      <c r="J172" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="K172" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L172" s="50"/>
+    </row>
+    <row r="173" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="50" t="n">
+        <v>2120</v>
+      </c>
+      <c r="B173" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C173" s="51"/>
+      <c r="D173" s="52"/>
+      <c r="E173" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F173" s="60" t="s">
+        <v>370</v>
+      </c>
+      <c r="G173" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H173" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I173" s="50" t="n">
+        <v>122017008</v>
+      </c>
+      <c r="J173" s="50" t="s">
+        <v>371</v>
+      </c>
+      <c r="K173" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L173" s="50"/>
+    </row>
+    <row r="174" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="50" t="n">
+        <v>2121</v>
+      </c>
+      <c r="B174" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C174" s="51"/>
+      <c r="D174" s="52"/>
+      <c r="E174" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F174" s="60" t="s">
+        <v>372</v>
+      </c>
+      <c r="G174" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H174" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I174" s="50" t="n">
+        <v>57582005</v>
+      </c>
+      <c r="J174" s="50" t="s">
+        <v>373</v>
+      </c>
+      <c r="K174" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L174" s="50"/>
+    </row>
+    <row r="175" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="50" t="n">
+        <v>2122</v>
+      </c>
+      <c r="B175" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C175" s="51"/>
+      <c r="D175" s="52"/>
+      <c r="E175" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F175" s="60" t="s">
+        <v>374</v>
+      </c>
+      <c r="G175" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H175" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I175" s="50" t="n">
+        <v>121602006</v>
+      </c>
+      <c r="J175" s="50" t="s">
+        <v>375</v>
+      </c>
+      <c r="K175" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L175" s="50"/>
+    </row>
+    <row r="176" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="50" t="n">
+        <v>2123</v>
+      </c>
+      <c r="B176" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C176" s="51"/>
+      <c r="D176" s="52"/>
+      <c r="E176" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F176" s="60" t="s">
+        <v>376</v>
+      </c>
+      <c r="G176" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H176" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I176" s="50" t="n">
+        <v>55112008</v>
+      </c>
+      <c r="J176" s="50" t="s">
+        <v>377</v>
+      </c>
+      <c r="K176" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L176" s="50"/>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="62"/>
+      <c r="B177" s="63"/>
+      <c r="C177" s="63"/>
+      <c r="D177" s="64"/>
+      <c r="E177" s="62"/>
+      <c r="F177" s="65"/>
+      <c r="G177" s="62"/>
+      <c r="H177" s="62"/>
+      <c r="I177" s="62"/>
+      <c r="J177" s="62"/>
+      <c r="K177" s="62"/>
+      <c r="L177" s="62"/>
+    </row>
+    <row r="178" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="50" t="n">
+        <v>2125</v>
+      </c>
+      <c r="B178" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C178" s="51"/>
+      <c r="D178" s="52"/>
+      <c r="E178" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F178" s="60" t="s">
+        <v>378</v>
+      </c>
+      <c r="G178" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H178" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I178" s="50" t="n">
+        <v>105336005</v>
+      </c>
+      <c r="J178" s="50" t="s">
+        <v>379</v>
+      </c>
+      <c r="K178" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L178" s="50"/>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="62"/>
+      <c r="B179" s="63"/>
+      <c r="C179" s="63"/>
+      <c r="D179" s="64"/>
+      <c r="E179" s="62"/>
+      <c r="F179" s="65"/>
+      <c r="G179" s="62"/>
+      <c r="H179" s="62"/>
+      <c r="I179" s="62"/>
+      <c r="J179" s="62"/>
+      <c r="K179" s="62"/>
+      <c r="L179" s="62"/>
+    </row>
+    <row r="180" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="50" t="n">
+        <v>2127</v>
+      </c>
+      <c r="B180" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C180" s="51"/>
+      <c r="D180" s="52"/>
+      <c r="E180" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F180" s="60" t="s">
+        <v>380</v>
+      </c>
+      <c r="G180" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H180" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I180" s="50" t="n">
+        <v>69285004</v>
+      </c>
+      <c r="J180" s="50" t="s">
+        <v>381</v>
+      </c>
+      <c r="K180" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L180" s="50"/>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="62"/>
+      <c r="B181" s="63"/>
+      <c r="C181" s="63"/>
+      <c r="D181" s="64"/>
+      <c r="E181" s="62"/>
+      <c r="F181" s="65"/>
+      <c r="G181" s="62"/>
+      <c r="H181" s="62"/>
+      <c r="I181" s="62"/>
+      <c r="J181" s="62"/>
+      <c r="K181" s="62"/>
+      <c r="L181" s="62"/>
+    </row>
+    <row r="182" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="50" t="n">
+        <v>2129</v>
+      </c>
+      <c r="B182" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C182" s="51"/>
+      <c r="D182" s="52"/>
+      <c r="E182" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F182" s="60" t="s">
+        <v>382</v>
+      </c>
+      <c r="G182" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H182" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I182" s="50" t="n">
+        <v>81410005</v>
+      </c>
+      <c r="J182" s="50" t="s">
+        <v>383</v>
+      </c>
+      <c r="K182" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L182" s="50"/>
+    </row>
+    <row r="183" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="50" t="n">
+        <v>2130</v>
+      </c>
+      <c r="B183" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C183" s="51"/>
+      <c r="D183" s="52"/>
+      <c r="E183" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F183" s="60" t="s">
+        <v>384</v>
+      </c>
+      <c r="G183" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H183" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I183" s="50" t="n">
+        <v>43388004</v>
+      </c>
+      <c r="J183" s="50" t="s">
+        <v>385</v>
+      </c>
+      <c r="K183" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L183" s="50"/>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="62"/>
+      <c r="B184" s="63"/>
+      <c r="C184" s="63"/>
+      <c r="D184" s="64"/>
+      <c r="E184" s="62"/>
+      <c r="F184" s="65"/>
+      <c r="G184" s="62"/>
+      <c r="H184" s="62"/>
+      <c r="I184" s="62"/>
+      <c r="J184" s="62"/>
+      <c r="K184" s="62"/>
+      <c r="L184" s="62"/>
+    </row>
+    <row r="185" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="50" t="n">
+        <v>2132</v>
+      </c>
+      <c r="B185" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C185" s="51"/>
+      <c r="D185" s="52"/>
+      <c r="E185" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F185" s="60" t="s">
+        <v>386</v>
+      </c>
+      <c r="G185" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H185" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I185" s="50" t="n">
+        <v>122349003</v>
+      </c>
+      <c r="J185" s="50" t="s">
+        <v>387</v>
+      </c>
+      <c r="K185" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L185" s="50"/>
+    </row>
+    <row r="186" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="50" t="n">
+        <v>2133</v>
+      </c>
+      <c r="B186" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C186" s="51"/>
+      <c r="D186" s="52"/>
+      <c r="E186" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F186" s="60" t="s">
+        <v>388</v>
+      </c>
+      <c r="G186" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H186" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I186" s="50" t="n">
+        <v>121603001</v>
+      </c>
+      <c r="J186" s="50" t="s">
+        <v>389</v>
+      </c>
+      <c r="K186" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L186" s="50"/>
+    </row>
+    <row r="187" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="50" t="n">
+        <v>2134</v>
+      </c>
+      <c r="B187" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C187" s="51"/>
+      <c r="D187" s="52"/>
+      <c r="E187" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F187" s="60" t="s">
+        <v>390</v>
+      </c>
+      <c r="G187" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H187" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I187" s="50" t="n">
+        <v>56919009</v>
+      </c>
+      <c r="J187" s="50" t="s">
+        <v>391</v>
+      </c>
+      <c r="K187" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L187" s="50"/>
+    </row>
+    <row r="188" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="50" t="n">
+        <v>2135</v>
+      </c>
+      <c r="B188" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C188" s="51"/>
+      <c r="D188" s="52"/>
+      <c r="E188" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F188" s="60" t="s">
+        <v>392</v>
+      </c>
+      <c r="G188" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H188" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I188" s="50" t="n">
+        <v>64685008</v>
+      </c>
+      <c r="J188" s="50" t="s">
+        <v>393</v>
+      </c>
+      <c r="K188" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L188" s="50"/>
+    </row>
+    <row r="189" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="50" t="n">
+        <v>2136</v>
+      </c>
+      <c r="B189" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C189" s="51"/>
+      <c r="D189" s="52"/>
+      <c r="E189" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F189" s="60" t="s">
+        <v>394</v>
+      </c>
+      <c r="G189" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H189" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I189" s="50" t="n">
+        <v>105131008</v>
+      </c>
+      <c r="J189" s="50" t="s">
+        <v>395</v>
+      </c>
+      <c r="K189" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L189" s="50"/>
+    </row>
+    <row r="190" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="50" t="n">
+        <v>2137</v>
+      </c>
+      <c r="B190" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C190" s="51"/>
+      <c r="D190" s="52"/>
+      <c r="E190" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F190" s="60" t="s">
+        <v>396</v>
+      </c>
+      <c r="G190" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H190" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I190" s="50" t="n">
+        <v>121505002</v>
+      </c>
+      <c r="J190" s="50" t="s">
+        <v>397</v>
+      </c>
+      <c r="K190" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L190" s="50"/>
+    </row>
+    <row r="191" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="50" t="n">
+        <v>2138</v>
+      </c>
+      <c r="B191" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C191" s="51"/>
+      <c r="D191" s="52"/>
+      <c r="E191" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F191" s="60" t="s">
+        <v>398</v>
+      </c>
+      <c r="G191" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H191" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I191" s="50" t="n">
+        <v>32464007</v>
+      </c>
+      <c r="J191" s="50" t="s">
+        <v>399</v>
+      </c>
+      <c r="K191" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L191" s="50"/>
+    </row>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="62"/>
+      <c r="B192" s="63"/>
+      <c r="C192" s="63"/>
+      <c r="D192" s="64"/>
+      <c r="E192" s="62"/>
+      <c r="F192" s="65"/>
+      <c r="G192" s="62"/>
+      <c r="H192" s="62"/>
+      <c r="I192" s="62"/>
+      <c r="J192" s="62"/>
+      <c r="K192" s="62"/>
+      <c r="L192" s="62"/>
+    </row>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="62"/>
+      <c r="B193" s="63"/>
+      <c r="C193" s="63"/>
+      <c r="D193" s="64"/>
+      <c r="E193" s="62"/>
+      <c r="F193" s="65"/>
+      <c r="G193" s="62"/>
+      <c r="H193" s="62"/>
+      <c r="I193" s="62"/>
+      <c r="J193" s="62"/>
+      <c r="K193" s="62"/>
+      <c r="L193" s="62"/>
+    </row>
+    <row r="194" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="50" t="n">
+        <v>2141</v>
+      </c>
+      <c r="B194" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C194" s="51"/>
+      <c r="D194" s="52"/>
+      <c r="E194" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F194" s="60" t="s">
+        <v>400</v>
+      </c>
+      <c r="G194" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H194" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I194" s="50" t="n">
+        <v>61065009</v>
+      </c>
+      <c r="J194" s="50" t="s">
+        <v>401</v>
+      </c>
+      <c r="K194" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L194" s="50"/>
+    </row>
+    <row r="195" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="50" t="n">
+        <v>2142</v>
+      </c>
+      <c r="B195" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C195" s="51"/>
+      <c r="D195" s="52"/>
+      <c r="E195" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F195" s="60" t="s">
+        <v>402</v>
+      </c>
+      <c r="G195" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H195" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I195" s="50" t="n">
+        <v>30200007</v>
+      </c>
+      <c r="J195" s="50" t="s">
+        <v>403</v>
+      </c>
+      <c r="K195" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L195" s="50"/>
+    </row>
+    <row r="196" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="50" t="n">
+        <v>2143</v>
+      </c>
+      <c r="B196" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C196" s="51"/>
+      <c r="D196" s="52"/>
+      <c r="E196" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F196" s="60" t="s">
+        <v>404</v>
+      </c>
+      <c r="G196" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H196" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I196" s="50" t="n">
+        <v>122350003</v>
+      </c>
+      <c r="J196" s="50" t="s">
+        <v>405</v>
+      </c>
+      <c r="K196" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L196" s="50"/>
+    </row>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="62"/>
+      <c r="B197" s="63"/>
+      <c r="C197" s="63"/>
+      <c r="D197" s="64"/>
+      <c r="E197" s="62"/>
+      <c r="F197" s="65"/>
+      <c r="G197" s="62"/>
+      <c r="H197" s="62"/>
+      <c r="I197" s="62"/>
+      <c r="J197" s="62"/>
+      <c r="K197" s="62"/>
+      <c r="L197" s="62"/>
+    </row>
+    <row r="198" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="50" t="n">
+        <v>2145</v>
+      </c>
+      <c r="B198" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C198" s="51"/>
+      <c r="D198" s="52"/>
+      <c r="E198" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F198" s="60" t="s">
+        <v>406</v>
+      </c>
+      <c r="G198" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H198" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I198" s="50" t="n">
+        <v>54392006</v>
+      </c>
+      <c r="J198" s="50" t="s">
+        <v>407</v>
+      </c>
+      <c r="K198" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L198" s="50"/>
+    </row>
+    <row r="199" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="50" t="n">
+        <v>2146</v>
+      </c>
+      <c r="B199" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C199" s="51"/>
+      <c r="D199" s="52"/>
+      <c r="E199" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F199" s="60" t="s">
+        <v>408</v>
+      </c>
+      <c r="G199" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H199" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I199" s="50" t="n">
+        <v>105207008</v>
+      </c>
+      <c r="J199" s="50" t="s">
+        <v>409</v>
+      </c>
+      <c r="K199" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L199" s="50"/>
+    </row>
+    <row r="200" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="66" t="n">
+        <v>2147</v>
+      </c>
+      <c r="B200" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C200" s="51"/>
+      <c r="D200" s="52"/>
+      <c r="E200" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F200" s="60" t="s">
+        <v>410</v>
+      </c>
+      <c r="G200" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H200" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I200" s="50" t="n">
+        <v>117739006</v>
+      </c>
+      <c r="J200" s="50" t="s">
+        <v>411</v>
+      </c>
+      <c r="K200" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L200" s="50"/>
+    </row>
+    <row r="201" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="50" t="n">
+        <v>2148</v>
+      </c>
+      <c r="B201" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C201" s="51"/>
+      <c r="D201" s="52"/>
+      <c r="E201" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F201" s="60" t="s">
+        <v>412</v>
+      </c>
+      <c r="G201" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H201" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I201" s="50" t="n">
+        <v>80152001</v>
+      </c>
+      <c r="J201" s="50" t="s">
+        <v>413</v>
+      </c>
+      <c r="K201" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L201" s="50"/>
+    </row>
+    <row r="202" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="50" t="n">
+        <v>2149</v>
+      </c>
+      <c r="B202" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C202" s="51"/>
+      <c r="D202" s="52"/>
+      <c r="E202" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F202" s="60" t="s">
+        <v>414</v>
+      </c>
+      <c r="G202" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H202" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I202" s="50" t="n">
+        <v>122321005</v>
+      </c>
+      <c r="J202" s="50" t="s">
+        <v>415</v>
+      </c>
+      <c r="K202" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L202" s="50"/>
+    </row>
+    <row r="203" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="50" t="n">
+        <v>2150</v>
+      </c>
+      <c r="B203" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C203" s="51"/>
+      <c r="D203" s="52"/>
+      <c r="E203" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F203" s="60" t="s">
+        <v>416</v>
+      </c>
+      <c r="G203" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H203" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I203" s="50" t="n">
+        <v>105192003</v>
+      </c>
+      <c r="J203" s="50" t="s">
+        <v>417</v>
+      </c>
+      <c r="K203" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L203" s="50"/>
+    </row>
+    <row r="204" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="50" t="n">
+        <v>2151</v>
+      </c>
+      <c r="B204" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C204" s="51"/>
+      <c r="D204" s="52"/>
+      <c r="E204" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F204" s="60" t="s">
+        <v>418</v>
+      </c>
+      <c r="G204" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H204" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I204" s="50" t="n">
+        <v>36206007</v>
+      </c>
+      <c r="J204" s="50" t="s">
+        <v>419</v>
+      </c>
+      <c r="K204" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L204" s="50"/>
+    </row>
+    <row r="205" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="50" t="n">
+        <v>2152</v>
+      </c>
+      <c r="B205" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C205" s="51"/>
+      <c r="D205" s="52"/>
+      <c r="E205" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F205" s="60" t="s">
+        <v>420</v>
+      </c>
+      <c r="G205" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H205" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I205" s="50" t="n">
+        <v>420880005</v>
+      </c>
+      <c r="J205" s="50" t="s">
+        <v>421</v>
+      </c>
+      <c r="K205" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L205" s="50"/>
+    </row>
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="67"/>
+      <c r="B206" s="68"/>
+      <c r="C206" s="68"/>
+      <c r="D206" s="69"/>
+      <c r="E206" s="67"/>
+      <c r="F206" s="70"/>
+      <c r="G206" s="67"/>
+      <c r="H206" s="67"/>
+      <c r="I206" s="67"/>
+      <c r="J206" s="67"/>
+      <c r="K206" s="67"/>
+      <c r="L206" s="67"/>
+    </row>
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="67"/>
+      <c r="B207" s="68"/>
+      <c r="C207" s="68"/>
+      <c r="D207" s="69"/>
+      <c r="E207" s="67"/>
+      <c r="F207" s="70"/>
+      <c r="G207" s="67"/>
+      <c r="H207" s="67"/>
+      <c r="I207" s="67"/>
+      <c r="J207" s="67"/>
+      <c r="K207" s="67"/>
+      <c r="L207" s="67"/>
+    </row>
+    <row r="208" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="50" t="n">
+        <v>2155</v>
+      </c>
+      <c r="B208" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C208" s="51"/>
+      <c r="D208" s="52"/>
+      <c r="E208" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F208" s="60" t="s">
+        <v>422</v>
+      </c>
+      <c r="G208" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H208" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I208" s="50" t="n">
+        <v>121373009</v>
+      </c>
+      <c r="J208" s="50" t="s">
+        <v>423</v>
+      </c>
+      <c r="K208" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L208" s="50"/>
+    </row>
+    <row r="209" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="50" t="n">
+        <v>2156</v>
+      </c>
+      <c r="B209" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C209" s="51"/>
+      <c r="D209" s="52"/>
+      <c r="E209" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F209" s="60" t="s">
+        <v>424</v>
+      </c>
+      <c r="G209" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H209" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I209" s="50" t="n">
+        <v>122078009</v>
+      </c>
+      <c r="J209" s="50" t="s">
+        <v>425</v>
+      </c>
+      <c r="K209" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L209" s="50"/>
+    </row>
+    <row r="210" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="50" t="n">
+        <v>2157</v>
+      </c>
+      <c r="B210" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C210" s="51"/>
+      <c r="D210" s="52"/>
+      <c r="E210" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F210" s="60" t="s">
+        <v>426</v>
+      </c>
+      <c r="G210" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H210" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I210" s="50" t="n">
+        <v>71167000</v>
+      </c>
+      <c r="J210" s="50" t="s">
+        <v>427</v>
+      </c>
+      <c r="K210" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L210" s="50"/>
+    </row>
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="67"/>
+      <c r="B211" s="68"/>
+      <c r="C211" s="68"/>
+      <c r="D211" s="69"/>
+      <c r="E211" s="67"/>
+      <c r="F211" s="70"/>
+      <c r="G211" s="67"/>
+      <c r="H211" s="67"/>
+      <c r="I211" s="67"/>
+      <c r="J211" s="67"/>
+      <c r="K211" s="67"/>
+      <c r="L211" s="67"/>
+    </row>
+    <row r="212" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="50" t="n">
+        <v>2159</v>
+      </c>
+      <c r="B212" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C212" s="51"/>
+      <c r="D212" s="52"/>
+      <c r="E212" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F212" s="60" t="s">
+        <v>428</v>
+      </c>
+      <c r="G212" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H212" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I212" s="50" t="n">
+        <v>105217003</v>
+      </c>
+      <c r="J212" s="50" t="s">
+        <v>429</v>
+      </c>
+      <c r="K212" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L212" s="50"/>
+    </row>
+    <row r="213" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="50" t="n">
+        <v>2160</v>
+      </c>
+      <c r="B213" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C213" s="51"/>
+      <c r="D213" s="52"/>
+      <c r="E213" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F213" s="60" t="s">
+        <v>430</v>
+      </c>
+      <c r="G213" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H213" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I213" s="50" t="n">
+        <v>87407009</v>
+      </c>
+      <c r="J213" s="50" t="s">
+        <v>431</v>
+      </c>
+      <c r="K213" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L213" s="50"/>
+    </row>
+    <row r="214" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="50" t="n">
+        <v>2161</v>
+      </c>
+      <c r="B214" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C214" s="51"/>
+      <c r="D214" s="52"/>
+      <c r="E214" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F214" s="60" t="s">
+        <v>432</v>
+      </c>
+      <c r="G214" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H214" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I214" s="50" t="n">
+        <v>105206004</v>
+      </c>
+      <c r="J214" s="50" t="s">
+        <v>433</v>
+      </c>
+      <c r="K214" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L214" s="50"/>
+    </row>
+    <row r="215" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="66" t="n">
+        <v>2162</v>
+      </c>
+      <c r="B215" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C215" s="51"/>
+      <c r="D215" s="52"/>
+      <c r="E215" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F215" s="60" t="s">
+        <v>434</v>
+      </c>
+      <c r="G215" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H215" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I215" s="50" t="n">
+        <v>122017008</v>
+      </c>
+      <c r="J215" s="50" t="s">
+        <v>371</v>
+      </c>
+      <c r="K215" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L215" s="50"/>
+    </row>
+    <row r="216" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="50" t="n">
+        <v>2163</v>
+      </c>
+      <c r="B216" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C216" s="51"/>
+      <c r="D216" s="52"/>
+      <c r="E216" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F216" s="60" t="s">
+        <v>435</v>
+      </c>
+      <c r="G216" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H216" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I216" s="50" t="n">
+        <v>117739006</v>
+      </c>
+      <c r="J216" s="50" t="s">
+        <v>411</v>
+      </c>
+      <c r="K216" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L216" s="50"/>
+    </row>
+    <row r="217" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="50" t="n">
+        <v>2164</v>
+      </c>
+      <c r="B217" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C217" s="51"/>
+      <c r="D217" s="52"/>
+      <c r="E217" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F217" s="60" t="s">
+        <v>436</v>
+      </c>
+      <c r="G217" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H217" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I217" s="50" t="n">
+        <v>121914001</v>
+      </c>
+      <c r="J217" s="50" t="s">
+        <v>437</v>
+      </c>
+      <c r="K217" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L217" s="50"/>
+    </row>
+    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="62"/>
+      <c r="B218" s="63"/>
+      <c r="C218" s="63"/>
+      <c r="D218" s="64"/>
+      <c r="E218" s="62"/>
+      <c r="F218" s="65"/>
+      <c r="G218" s="62"/>
+      <c r="H218" s="62"/>
+      <c r="I218" s="62"/>
+      <c r="J218" s="62"/>
+      <c r="K218" s="62"/>
+      <c r="L218" s="62"/>
+    </row>
+    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="62"/>
+      <c r="B219" s="63"/>
+      <c r="C219" s="63"/>
+      <c r="D219" s="64"/>
+      <c r="E219" s="62"/>
+      <c r="F219" s="65"/>
+      <c r="G219" s="62"/>
+      <c r="H219" s="62"/>
+      <c r="I219" s="62"/>
+      <c r="J219" s="62"/>
+      <c r="K219" s="62"/>
+      <c r="L219" s="62"/>
+    </row>
+    <row r="220" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="50" t="n">
+        <v>2167</v>
+      </c>
+      <c r="B220" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C220" s="51"/>
+      <c r="D220" s="52"/>
+      <c r="E220" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F220" s="60" t="s">
+        <v>438</v>
+      </c>
+      <c r="G220" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H220" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I220" s="50" t="n">
+        <v>104311005</v>
+      </c>
+      <c r="J220" s="50" t="s">
+        <v>439</v>
+      </c>
+      <c r="K220" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L220" s="50"/>
+    </row>
+    <row r="221" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="50" t="n">
+        <v>2168</v>
+      </c>
+      <c r="B221" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C221" s="51"/>
+      <c r="D221" s="52"/>
+      <c r="E221" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F221" s="60" t="s">
+        <v>440</v>
+      </c>
+      <c r="G221" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H221" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I221" s="50" t="n">
+        <v>104325006</v>
+      </c>
+      <c r="J221" s="50" t="s">
+        <v>441</v>
+      </c>
+      <c r="K221" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L221" s="50"/>
+    </row>
+    <row r="222" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="50" t="n">
+        <v>2169</v>
+      </c>
+      <c r="B222" s="51" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C222" s="51"/>
+      <c r="D222" s="52"/>
+      <c r="E222" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F222" s="60" t="s">
+        <v>442</v>
+      </c>
+      <c r="G222" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H222" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I222" s="50" t="n">
+        <v>37538009</v>
+      </c>
+      <c r="J222" s="50" t="s">
+        <v>443</v>
+      </c>
+      <c r="K222" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L222" s="50"/>
+    </row>
+    <row r="223" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="50" t="n">
+        <v>2170</v>
+      </c>
+      <c r="B223" s="51" t="n">
+        <v>42140</v>
+      </c>
+      <c r="C223" s="51"/>
+      <c r="D223" s="52"/>
+      <c r="E223" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F223" s="60" t="s">
+        <v>444</v>
+      </c>
+      <c r="G223" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H223" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I223" s="50" t="n">
+        <v>62037009</v>
+      </c>
+      <c r="J223" s="50" t="s">
+        <v>445</v>
+      </c>
+      <c r="K223" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L223" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>